<commit_message>
Updated list of crypto coins on eToro
</commit_message>
<xml_diff>
--- a/Crypto_info.xlsx
+++ b/Crypto_info.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="85">
   <si>
     <t>Crypto name</t>
   </si>
@@ -56,9 +56,6 @@
     <t>BCH</t>
   </si>
   <si>
-    <t>Ripple</t>
-  </si>
-  <si>
     <t>XRP</t>
   </si>
   <si>
@@ -71,9 +68,6 @@
     <t>LTC</t>
   </si>
   <si>
-    <t>Ethereum Cash</t>
-  </si>
-  <si>
     <t>ETC</t>
   </si>
   <si>
@@ -120,6 +114,171 @@
   </si>
   <si>
     <t>XTZ</t>
+  </si>
+  <si>
+    <t>Ethereum Classic</t>
+  </si>
+  <si>
+    <t>Polkadot</t>
+  </si>
+  <si>
+    <t>DOT</t>
+  </si>
+  <si>
+    <t>Maker</t>
+  </si>
+  <si>
+    <t>MKR</t>
+  </si>
+  <si>
+    <t>Compound</t>
+  </si>
+  <si>
+    <t>COMP</t>
+  </si>
+  <si>
+    <t>Chainlink</t>
+  </si>
+  <si>
+    <t>LINK</t>
+  </si>
+  <si>
+    <t>Uniswap</t>
+  </si>
+  <si>
+    <t>UNI</t>
+  </si>
+  <si>
+    <t>Yearn.finance</t>
+  </si>
+  <si>
+    <t>YFI</t>
+  </si>
+  <si>
+    <t>Dogecoin</t>
+  </si>
+  <si>
+    <t>DOGE</t>
+  </si>
+  <si>
+    <t>Aave</t>
+  </si>
+  <si>
+    <t>AAVE</t>
+  </si>
+  <si>
+    <t>Filecoin</t>
+  </si>
+  <si>
+    <t>FIL</t>
+  </si>
+  <si>
+    <t>Algorand</t>
+  </si>
+  <si>
+    <t>ALGO</t>
+  </si>
+  <si>
+    <t>Cosmos</t>
+  </si>
+  <si>
+    <t>ATOM</t>
+  </si>
+  <si>
+    <t>Decentraland</t>
+  </si>
+  <si>
+    <t>MANA</t>
+  </si>
+  <si>
+    <t>Enjin</t>
+  </si>
+  <si>
+    <t>ENJ</t>
+  </si>
+  <si>
+    <t>Basic Attention Token</t>
+  </si>
+  <si>
+    <t>BAT</t>
+  </si>
+  <si>
+    <t>Polygon</t>
+  </si>
+  <si>
+    <t>MATIC</t>
+  </si>
+  <si>
+    <t>Spark</t>
+  </si>
+  <si>
+    <t>FLR</t>
+  </si>
+  <si>
+    <t>Chiliz</t>
+  </si>
+  <si>
+    <t>CHZ</t>
+  </si>
+  <si>
+    <t>Solana</t>
+  </si>
+  <si>
+    <t>SOL</t>
+  </si>
+  <si>
+    <t>The Graph</t>
+  </si>
+  <si>
+    <t>GRT</t>
+  </si>
+  <si>
+    <t>1inch</t>
+  </si>
+  <si>
+    <t>1INCH</t>
+  </si>
+  <si>
+    <t>Curve</t>
+  </si>
+  <si>
+    <t>CRV</t>
+  </si>
+  <si>
+    <t>Celo</t>
+  </si>
+  <si>
+    <t>CELO</t>
+  </si>
+  <si>
+    <t>SushiSwap</t>
+  </si>
+  <si>
+    <t>SUSHI</t>
+  </si>
+  <si>
+    <t>Quant</t>
+  </si>
+  <si>
+    <t>QNT</t>
+  </si>
+  <si>
+    <t>Shiba (in millions)</t>
+  </si>
+  <si>
+    <t>SHIBxM</t>
+  </si>
+  <si>
+    <t>Axie Infinity</t>
+  </si>
+  <si>
+    <t>AXS</t>
+  </si>
+  <si>
+    <t>SAND</t>
+  </si>
+  <si>
+    <t>The Sandbox</t>
   </si>
 </sst>
 </file>
@@ -176,8 +335,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A1:B17" totalsRowShown="0">
-  <autoFilter ref="A1:B17"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A1:B44" totalsRowShown="0">
+  <autoFilter ref="A1:B44"/>
   <sortState ref="A2:B17">
     <sortCondition ref="A1"/>
   </sortState>
@@ -452,16 +611,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B17"/>
+  <dimension ref="A1:B44"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="E41" sqref="E41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" customWidth="1"/>
-    <col min="2" max="2" width="9.7109375" customWidth="1"/>
+    <col min="1" max="1" width="26" customWidth="1"/>
+    <col min="2" max="2" width="15.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -474,18 +633,18 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>28</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>29</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -498,106 +657,322 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="B5" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
       <c r="B7" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="B8" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="B9" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B10" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="B11" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B12" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="B13" t="s">
-        <v>11</v>
+        <v>21</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B14" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B15" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B16" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B17" t="s">
-        <v>27</v>
+        <v>29</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>31</v>
+      </c>
+      <c r="B18" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>33</v>
+      </c>
+      <c r="B19" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>35</v>
+      </c>
+      <c r="B20" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>37</v>
+      </c>
+      <c r="B21" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>39</v>
+      </c>
+      <c r="B22" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>41</v>
+      </c>
+      <c r="B23" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>43</v>
+      </c>
+      <c r="B24" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>45</v>
+      </c>
+      <c r="B25" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>47</v>
+      </c>
+      <c r="B26" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>49</v>
+      </c>
+      <c r="B27" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>51</v>
+      </c>
+      <c r="B28" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>53</v>
+      </c>
+      <c r="B29" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>55</v>
+      </c>
+      <c r="B30" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>57</v>
+      </c>
+      <c r="B31" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>59</v>
+      </c>
+      <c r="B32" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>61</v>
+      </c>
+      <c r="B33" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>63</v>
+      </c>
+      <c r="B34" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>65</v>
+      </c>
+      <c r="B35" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>67</v>
+      </c>
+      <c r="B36" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>69</v>
+      </c>
+      <c r="B37" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>71</v>
+      </c>
+      <c r="B38" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>73</v>
+      </c>
+      <c r="B39" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>75</v>
+      </c>
+      <c r="B40" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>77</v>
+      </c>
+      <c r="B41" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>79</v>
+      </c>
+      <c r="B42" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>81</v>
+      </c>
+      <c r="B43" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>83</v>
+      </c>
+      <c r="B44" t="s">
+        <v>84</v>
       </c>
     </row>
   </sheetData>

</xml_diff>